<commit_message>
Updated Code and Cleaned up Data
</commit_message>
<xml_diff>
--- a/Data/Sperm_Abnormality_Database.xlsx
+++ b/Data/Sperm_Abnormality_Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/nozo0116_student_ubc_ca/Documents/Quantitative_Ecology_Lab/Nozomu_Hirama_Undergraduate_Honours/Mammalian_Sperm_Abnormality/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{3A57838B-7E2E-7345-9921-EA813EEEE4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{24E349AB-55EC-1A4C-94C7-371599F4A982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9100" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sperm_Abnormality_Database" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2031" uniqueCount="777">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1999" uniqueCount="758">
   <si>
     <t>Binomial</t>
   </si>
@@ -1071,12 +1071,6 @@
     <t>Plecturocebus grovesi</t>
   </si>
   <si>
-    <t>True's Beaked Whale</t>
-  </si>
-  <si>
-    <t>Mesoplodon mirus</t>
-  </si>
-  <si>
     <t>Hose's Palm Civet</t>
   </si>
   <si>
@@ -1197,12 +1191,6 @@
     <t>Crocidura nigeriae</t>
   </si>
   <si>
-    <t>Fin Whale</t>
-  </si>
-  <si>
-    <t>Balaenoptera physalus</t>
-  </si>
-  <si>
     <t>Common Dwarf Mongoose</t>
   </si>
   <si>
@@ -1245,12 +1233,6 @@
     <t>Saguinus weddelli</t>
   </si>
   <si>
-    <t>Australian Humpback Dolphin</t>
-  </si>
-  <si>
-    <t>Sousa sahulensis</t>
-  </si>
-  <si>
     <t>Urubamba Brown Titi</t>
   </si>
   <si>
@@ -1368,12 +1350,6 @@
     <t>Sylvisorex akaibei</t>
   </si>
   <si>
-    <t>Tucuxi</t>
-  </si>
-  <si>
-    <t>Sotalia fluviatilis</t>
-  </si>
-  <si>
     <t>Central African Potto</t>
   </si>
   <si>
@@ -1392,12 +1368,6 @@
     <t>Sylvisorex howelli</t>
   </si>
   <si>
-    <t>Harbor Porpoise</t>
-  </si>
-  <si>
-    <t>Phocoena phocoena</t>
-  </si>
-  <si>
     <t>Hidden Brown-toothed Shrew</t>
   </si>
   <si>
@@ -1674,15 +1644,6 @@
     <t>Kobus megaceros</t>
   </si>
   <si>
-    <t>Bryde's Whale</t>
-  </si>
-  <si>
-    <t>Balaenoptera brydei</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1262/jrd.50.419</t>
-  </si>
-  <si>
     <t>Greater Forest Shrew</t>
   </si>
   <si>
@@ -1953,12 +1914,6 @@
     <t>Otocyon megalotis</t>
   </si>
   <si>
-    <t>Arnoux's Beaked Whale</t>
-  </si>
-  <si>
-    <t>Berardius arnuxii</t>
-  </si>
-  <si>
     <t>Harenna White-toothed Shrew</t>
   </si>
   <si>
@@ -1995,12 +1950,6 @@
     <t>Tarsius tumpara</t>
   </si>
   <si>
-    <t>Amazon River Dolphin</t>
-  </si>
-  <si>
-    <t>Inia geoffrensis</t>
-  </si>
-  <si>
     <t>Ecuadorean Tapeti</t>
   </si>
   <si>
@@ -2206,12 +2155,6 @@
   </si>
   <si>
     <t>Marmosops incanus</t>
-  </si>
-  <si>
-    <t>Baiji</t>
-  </si>
-  <si>
-    <t>Lipotes vexillifer</t>
   </si>
   <si>
     <t>Jalisco Shrew</t>
@@ -3259,8 +3202,8 @@
   <dimension ref="A1:AL501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D301" sqref="D301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3391,7 +3334,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>752</v>
+        <v>733</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -3536,7 +3479,7 @@
         <v>12</v>
       </c>
       <c r="AC3" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="AL3" s="6"/>
     </row>
@@ -4935,7 +4878,7 @@
         <v>12</v>
       </c>
       <c r="AC24" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="AL24" s="6"/>
     </row>
@@ -5144,7 +5087,7 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>765</v>
+        <v>746</v>
       </c>
       <c r="D28" t="s">
         <v>80</v>
@@ -7276,7 +7219,7 @@
         <v>146</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>766</v>
+        <v>747</v>
       </c>
       <c r="D62" t="s">
         <v>80</v>
@@ -7336,7 +7279,7 @@
         <v>146</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>766</v>
+        <v>747</v>
       </c>
       <c r="D63" t="s">
         <v>80</v>
@@ -7951,10 +7894,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>769</v>
+        <v>750</v>
       </c>
       <c r="C74" t="s">
-        <v>770</v>
+        <v>751</v>
       </c>
       <c r="D74" t="s">
         <v>81</v>
@@ -10354,15 +10297,7 @@
       <c r="A147">
         <v>146</v>
       </c>
-      <c r="B147" t="s">
-        <v>344</v>
-      </c>
-      <c r="C147" t="s">
-        <v>345</v>
-      </c>
-      <c r="D147" t="s">
-        <v>81</v>
-      </c>
+      <c r="D147"/>
       <c r="G147"/>
       <c r="R147"/>
       <c r="S147"/>
@@ -10373,10 +10308,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>771</v>
+        <v>752</v>
       </c>
       <c r="C148" t="s">
-        <v>772</v>
+        <v>753</v>
       </c>
       <c r="D148" t="s">
         <v>81</v>
@@ -10391,10 +10326,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C149" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D149" t="s">
         <v>81</v>
@@ -10409,10 +10344,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C150" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D150" t="s">
         <v>80</v>
@@ -10430,7 +10365,7 @@
         <v>2003-08-31</v>
       </c>
       <c r="I150" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J150" t="s">
         <v>57</v>
@@ -10454,7 +10389,7 @@
       </c>
       <c r="AA150"/>
       <c r="AB150" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="151" spans="1:29" x14ac:dyDescent="0.2">
@@ -10462,10 +10397,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C151" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D151" t="s">
         <v>80</v>
@@ -10481,10 +10416,10 @@
       <c r="S151"/>
       <c r="AA151"/>
       <c r="AB151" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AC151" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.2">
@@ -10492,10 +10427,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C152" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D152" t="s">
         <v>80</v>
@@ -10544,10 +10479,10 @@
         <v>9</v>
       </c>
       <c r="AA152" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AB152" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="153" spans="1:29" x14ac:dyDescent="0.2">
@@ -10555,10 +10490,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C153" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D153" t="s">
         <v>80</v>
@@ -10571,7 +10506,7 @@
       </c>
       <c r="G153"/>
       <c r="I153" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J153">
         <v>31.210685770000001</v>
@@ -10610,7 +10545,7 @@
         <v>59</v>
       </c>
       <c r="AB153" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="154" spans="1:29" x14ac:dyDescent="0.2">
@@ -10618,10 +10553,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C154" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D154" t="s">
         <v>80</v>
@@ -10637,10 +10572,10 @@
       <c r="S154"/>
       <c r="AA154"/>
       <c r="AB154" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="AC154" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="155" spans="1:29" x14ac:dyDescent="0.2">
@@ -10648,10 +10583,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C155" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D155" t="s">
         <v>80</v>
@@ -10686,7 +10621,7 @@
         <v>59</v>
       </c>
       <c r="AB155" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="156" spans="1:29" x14ac:dyDescent="0.2">
@@ -10694,10 +10629,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C156" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D156" t="s">
         <v>80</v>
@@ -10710,7 +10645,7 @@
       </c>
       <c r="G156"/>
       <c r="I156" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J156">
         <v>-2.5416327189999999</v>
@@ -10741,7 +10676,7 @@
         <v>59</v>
       </c>
       <c r="AB156" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="157" spans="1:29" x14ac:dyDescent="0.2">
@@ -10749,10 +10684,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C157" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D157" t="s">
         <v>80</v>
@@ -10802,7 +10737,7 @@
       </c>
       <c r="AA157"/>
       <c r="AB157" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="158" spans="1:29" x14ac:dyDescent="0.2">
@@ -10810,10 +10745,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C158" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D158" t="s">
         <v>81</v>
@@ -10828,10 +10763,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C159" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D159" t="s">
         <v>81</v>
@@ -10846,10 +10781,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C160" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D160" t="s">
         <v>81</v>
@@ -10864,10 +10799,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C161" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D161" t="s">
         <v>81</v>
@@ -10882,10 +10817,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C162" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D162" t="s">
         <v>81</v>
@@ -10900,10 +10835,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C163" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D163" t="s">
         <v>81</v>
@@ -10918,10 +10853,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C164" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D164" t="s">
         <v>81</v>
@@ -10936,10 +10871,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C165" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D165" t="s">
         <v>81</v>
@@ -10954,10 +10889,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C166" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D166" t="s">
         <v>81</v>
@@ -10972,10 +10907,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C167" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D167" t="s">
         <v>81</v>
@@ -10990,10 +10925,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C168" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D168" t="s">
         <v>81</v>
@@ -11008,10 +10943,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>773</v>
+        <v>754</v>
       </c>
       <c r="C169" t="s">
-        <v>774</v>
+        <v>755</v>
       </c>
       <c r="D169" t="s">
         <v>81</v>
@@ -11025,15 +10960,7 @@
       <c r="A170">
         <v>169</v>
       </c>
-      <c r="B170" t="s">
-        <v>386</v>
-      </c>
-      <c r="C170" t="s">
-        <v>387</v>
-      </c>
-      <c r="D170" t="s">
-        <v>81</v>
-      </c>
+      <c r="D170"/>
       <c r="G170"/>
       <c r="R170"/>
       <c r="S170"/>
@@ -11044,10 +10971,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C171" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D171" t="s">
         <v>81</v>
@@ -11062,10 +10989,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C172" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D172" t="s">
         <v>81</v>
@@ -11080,10 +11007,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C173" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D173" t="s">
         <v>81</v>
@@ -11098,10 +11025,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C174" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D174" t="s">
         <v>81</v>
@@ -11116,10 +11043,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C175" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D175" t="s">
         <v>81</v>
@@ -11134,10 +11061,10 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C176" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D176" t="s">
         <v>81</v>
@@ -11152,10 +11079,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>775</v>
+        <v>756</v>
       </c>
       <c r="C177" t="s">
-        <v>776</v>
+        <v>757</v>
       </c>
       <c r="D177" t="s">
         <v>81</v>
@@ -11170,10 +11097,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C178" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D178" t="s">
         <v>81</v>
@@ -11187,15 +11114,7 @@
       <c r="A179">
         <v>178</v>
       </c>
-      <c r="B179" t="s">
-        <v>402</v>
-      </c>
-      <c r="C179" t="s">
-        <v>403</v>
-      </c>
-      <c r="D179" t="s">
-        <v>81</v>
-      </c>
+      <c r="D179"/>
       <c r="G179"/>
       <c r="R179"/>
       <c r="S179"/>
@@ -11206,10 +11125,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C180" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D180" t="s">
         <v>81</v>
@@ -11224,10 +11143,10 @@
         <v>180</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="D181" t="s">
         <v>80</v>
@@ -11264,7 +11183,7 @@
       </c>
       <c r="AA181"/>
       <c r="AB181" s="2" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="182" spans="1:29" x14ac:dyDescent="0.2">
@@ -11272,10 +11191,10 @@
         <v>181</v>
       </c>
       <c r="B182" s="10" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D182" t="s">
         <v>81</v>
@@ -11290,10 +11209,10 @@
         <v>182</v>
       </c>
       <c r="B183" s="10" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D183" t="s">
         <v>81</v>
@@ -11308,10 +11227,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="10" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D184" t="s">
         <v>81</v>
@@ -11326,10 +11245,10 @@
         <v>184</v>
       </c>
       <c r="B185" s="10" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="D185" t="s">
         <v>81</v>
@@ -11344,10 +11263,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="D186" t="s">
         <v>81</v>
@@ -11362,10 +11281,10 @@
         <v>186</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C187" s="10" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D187" t="s">
         <v>81</v>
@@ -11380,10 +11299,10 @@
         <v>187</v>
       </c>
       <c r="B188" s="10" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D188" t="s">
         <v>81</v>
@@ -11416,7 +11335,7 @@
         <v>1996-01-01</v>
       </c>
       <c r="I189" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="J189" t="s">
         <v>57</v>
@@ -11476,7 +11395,7 @@
         <v>100</v>
       </c>
       <c r="AB189" s="2" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="190" spans="1:29" x14ac:dyDescent="0.2">
@@ -11500,7 +11419,7 @@
       </c>
       <c r="G190"/>
       <c r="I190" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="J190" t="s">
         <v>57</v>
@@ -11520,10 +11439,10 @@
       </c>
       <c r="AA190"/>
       <c r="AB190" s="2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="AC190" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="191" spans="1:29" x14ac:dyDescent="0.2">
@@ -11547,7 +11466,7 @@
       </c>
       <c r="G191"/>
       <c r="I191" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="J191" t="s">
         <v>57</v>
@@ -11567,10 +11486,10 @@
       </c>
       <c r="AA191"/>
       <c r="AB191" s="2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="AC191" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="192" spans="1:29" x14ac:dyDescent="0.2">
@@ -11590,10 +11509,10 @@
         <v>192</v>
       </c>
       <c r="B193" s="10" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D193" t="s">
         <v>81</v>
@@ -11608,10 +11527,10 @@
         <v>193</v>
       </c>
       <c r="B194" s="10" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D194" t="s">
         <v>81</v>
@@ -11626,10 +11545,10 @@
         <v>194</v>
       </c>
       <c r="B195" s="10" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="C195" s="10" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D195" t="s">
         <v>81</v>
@@ -11644,10 +11563,10 @@
         <v>195</v>
       </c>
       <c r="B196" s="10" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="C196" s="10" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="D196" t="s">
         <v>81</v>
@@ -11662,10 +11581,10 @@
         <v>196</v>
       </c>
       <c r="B197" s="10" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="C197" s="10" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="D197" t="s">
         <v>81</v>
@@ -11680,10 +11599,10 @@
         <v>197</v>
       </c>
       <c r="B198" s="10" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="C198" s="10" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D198" t="s">
         <v>81</v>
@@ -11698,10 +11617,10 @@
         <v>198</v>
       </c>
       <c r="B199" s="10" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D199" t="s">
         <v>81</v>
@@ -11715,15 +11634,9 @@
       <c r="A200">
         <v>199</v>
       </c>
-      <c r="B200" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="C200" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="D200" t="s">
-        <v>81</v>
-      </c>
+      <c r="B200" s="10"/>
+      <c r="C200" s="10"/>
+      <c r="D200"/>
       <c r="G200"/>
       <c r="R200"/>
       <c r="S200"/>
@@ -11734,10 +11647,10 @@
         <v>200</v>
       </c>
       <c r="B201" s="10" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="C201" s="10" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="D201" t="s">
         <v>81</v>
@@ -11752,10 +11665,10 @@
         <v>201</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C202" s="10" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D202" t="s">
         <v>81</v>
@@ -11770,10 +11683,10 @@
         <v>202</v>
       </c>
       <c r="B203" s="10" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="C203" s="10" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="D203" t="s">
         <v>81</v>
@@ -11787,15 +11700,9 @@
       <c r="A204">
         <v>203</v>
       </c>
-      <c r="B204" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="C204" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="D204" t="s">
-        <v>81</v>
-      </c>
+      <c r="B204" s="10"/>
+      <c r="C204" s="10"/>
+      <c r="D204"/>
       <c r="G204"/>
       <c r="R204"/>
       <c r="S204"/>
@@ -11806,10 +11713,10 @@
         <v>204</v>
       </c>
       <c r="B205" s="10" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="C205" s="10" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="D205" t="s">
         <v>81</v>
@@ -11824,10 +11731,10 @@
         <v>205</v>
       </c>
       <c r="B206" s="10" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="C206" s="10" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="D206" t="s">
         <v>81</v>
@@ -11842,10 +11749,10 @@
         <v>206</v>
       </c>
       <c r="B207" s="10" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="C207" s="10" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="D207" t="s">
         <v>81</v>
@@ -11860,10 +11767,10 @@
         <v>207</v>
       </c>
       <c r="B208" s="10" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="C208" s="10" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D208" t="s">
         <v>81</v>
@@ -11878,10 +11785,10 @@
         <v>208</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="C209" s="10" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="D209" t="s">
         <v>81</v>
@@ -11896,10 +11803,10 @@
         <v>209</v>
       </c>
       <c r="B210" s="10" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="C210" s="10" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="D210" t="s">
         <v>81</v>
@@ -11914,10 +11821,10 @@
         <v>210</v>
       </c>
       <c r="B211" s="10" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="C211" s="10" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="D211" t="s">
         <v>81</v>
@@ -11932,10 +11839,10 @@
         <v>211</v>
       </c>
       <c r="B212" s="10" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="C212" s="10" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D212" t="s">
         <v>81</v>
@@ -11950,10 +11857,10 @@
         <v>212</v>
       </c>
       <c r="B213" s="10" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="C213" s="10" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="D213" t="s">
         <v>81</v>
@@ -11968,10 +11875,10 @@
         <v>213</v>
       </c>
       <c r="B214" s="10" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="C214" s="10" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="D214" t="s">
         <v>81</v>
@@ -11986,10 +11893,10 @@
         <v>214</v>
       </c>
       <c r="B215" s="10" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="C215" s="10" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="D215" t="s">
         <v>81</v>
@@ -12004,10 +11911,10 @@
         <v>215</v>
       </c>
       <c r="B216" s="10" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="C216" s="10" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="D216" t="s">
         <v>81</v>
@@ -12022,10 +11929,10 @@
         <v>216</v>
       </c>
       <c r="B217" s="10" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="C217" s="10" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="D217" t="s">
         <v>81</v>
@@ -12040,10 +11947,10 @@
         <v>217</v>
       </c>
       <c r="B218" s="10" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="D218" t="s">
         <v>81</v>
@@ -12058,10 +11965,10 @@
         <v>218</v>
       </c>
       <c r="B219" s="10" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="C219" s="10" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="D219" t="s">
         <v>81</v>
@@ -12076,10 +11983,10 @@
         <v>219</v>
       </c>
       <c r="B220" s="10" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="C220" s="10" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="D220" t="s">
         <v>81</v>
@@ -12094,10 +12001,10 @@
         <v>220</v>
       </c>
       <c r="B221" s="10" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="C221" s="10" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="D221" t="s">
         <v>81</v>
@@ -12112,10 +12019,10 @@
         <v>221</v>
       </c>
       <c r="B222" s="10" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="C222" s="10" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="D222" t="s">
         <v>81</v>
@@ -12130,10 +12037,10 @@
         <v>222</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="D223" t="s">
         <v>81</v>
@@ -12148,10 +12055,10 @@
         <v>223</v>
       </c>
       <c r="B224" s="10" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="C224" s="10" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="D224" t="s">
         <v>81</v>
@@ -12166,10 +12073,10 @@
         <v>224</v>
       </c>
       <c r="B225" s="10" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="C225" s="10" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="D225" t="s">
         <v>81</v>
@@ -12184,10 +12091,10 @@
         <v>225</v>
       </c>
       <c r="B226" s="10" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="C226" s="10" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="D226" t="s">
         <v>81</v>
@@ -12202,10 +12109,10 @@
         <v>226</v>
       </c>
       <c r="B227" s="10" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="C227" s="10" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="D227" t="s">
         <v>81</v>
@@ -12220,10 +12127,10 @@
         <v>227</v>
       </c>
       <c r="B228" s="10" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="C228" s="10" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="D228" t="s">
         <v>81</v>
@@ -12238,10 +12145,10 @@
         <v>228</v>
       </c>
       <c r="B229" s="10" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="C229" s="10" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
       <c r="D229" t="s">
         <v>81</v>
@@ -12256,10 +12163,10 @@
         <v>229</v>
       </c>
       <c r="B230" s="10" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="C230" s="10" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="D230" t="s">
         <v>81</v>
@@ -12274,10 +12181,10 @@
         <v>230</v>
       </c>
       <c r="B231" s="10" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="C231" s="10" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="D231" t="s">
         <v>81</v>
@@ -12292,10 +12199,10 @@
         <v>231</v>
       </c>
       <c r="B232" s="10" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="C232" s="10" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="D232" t="s">
         <v>81</v>
@@ -12310,10 +12217,10 @@
         <v>232</v>
       </c>
       <c r="B233" s="10" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="C233" s="10" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="D233" t="s">
         <v>81</v>
@@ -12328,10 +12235,10 @@
         <v>233</v>
       </c>
       <c r="B234" s="10" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="C234" s="10" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="D234" t="s">
         <v>81</v>
@@ -12346,10 +12253,10 @@
         <v>234</v>
       </c>
       <c r="B235" s="10" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="C235" s="10" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="D235" t="s">
         <v>81</v>
@@ -12364,10 +12271,10 @@
         <v>235</v>
       </c>
       <c r="B236" s="10" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="C236" s="10" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="D236" t="s">
         <v>81</v>
@@ -12382,10 +12289,10 @@
         <v>236</v>
       </c>
       <c r="B237" s="10" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="C237" s="10" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="D237" t="s">
         <v>81</v>
@@ -12400,10 +12307,10 @@
         <v>237</v>
       </c>
       <c r="B238" s="10" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="C238" s="10" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="D238" t="s">
         <v>81</v>
@@ -12418,10 +12325,10 @@
         <v>238</v>
       </c>
       <c r="B239" s="10" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="C239" s="10" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="D239" t="s">
         <v>81</v>
@@ -12436,10 +12343,10 @@
         <v>239</v>
       </c>
       <c r="B240" s="10" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="C240" s="10" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="D240" t="s">
         <v>81</v>
@@ -12454,10 +12361,10 @@
         <v>240</v>
       </c>
       <c r="B241" s="10" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="C241" s="10" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="D241" t="s">
         <v>81</v>
@@ -12472,10 +12379,10 @@
         <v>241</v>
       </c>
       <c r="B242" s="10" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="C242" s="10" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="D242" t="s">
         <v>81</v>
@@ -12490,10 +12397,10 @@
         <v>242</v>
       </c>
       <c r="B243" s="10" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="C243" s="10" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="D243" t="s">
         <v>81</v>
@@ -12508,10 +12415,10 @@
         <v>243</v>
       </c>
       <c r="B244" s="10" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C244" s="10" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="D244" t="s">
         <v>81</v>
@@ -12526,10 +12433,10 @@
         <v>244</v>
       </c>
       <c r="B245" s="10" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C245" s="10" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="D245" t="s">
         <v>80</v>
@@ -12578,7 +12485,7 @@
         <v>65</v>
       </c>
       <c r="AB245" s="2" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
     </row>
     <row r="246" spans="1:28" x14ac:dyDescent="0.2">
@@ -12586,10 +12493,10 @@
         <v>245</v>
       </c>
       <c r="B246" s="10" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="C246" s="10" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="D246" t="s">
         <v>80</v>
@@ -12638,7 +12545,7 @@
         <v>57</v>
       </c>
       <c r="AB246" s="2" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
     </row>
     <row r="247" spans="1:28" x14ac:dyDescent="0.2">
@@ -12646,10 +12553,10 @@
         <v>246</v>
       </c>
       <c r="B247" s="10" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C247" s="10" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="D247" t="s">
         <v>80</v>
@@ -12701,13 +12608,13 @@
         <v>97</v>
       </c>
       <c r="Z247" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="AA247" t="s">
         <v>65</v>
       </c>
       <c r="AB247" s="2" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
     </row>
     <row r="248" spans="1:28" x14ac:dyDescent="0.2">
@@ -12715,10 +12622,10 @@
         <v>247</v>
       </c>
       <c r="B248" s="10" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="D248" t="s">
         <v>80</v>
@@ -12752,7 +12659,7 @@
       </c>
       <c r="AA248"/>
       <c r="AB248" s="2" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
     </row>
     <row r="249" spans="1:28" x14ac:dyDescent="0.2">
@@ -12760,10 +12667,10 @@
         <v>248</v>
       </c>
       <c r="B249" s="10" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C249" s="10" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="D249" t="s">
         <v>80</v>
@@ -12807,11 +12714,11 @@
         <v>95.25</v>
       </c>
       <c r="Z249" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="AA249"/>
       <c r="AB249" s="2" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
     </row>
     <row r="250" spans="1:28" x14ac:dyDescent="0.2">
@@ -12819,10 +12726,10 @@
         <v>249</v>
       </c>
       <c r="B250" s="10" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C250" s="10" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="D250" t="s">
         <v>80</v>
@@ -12872,7 +12779,7 @@
         <v>59</v>
       </c>
       <c r="AB250" s="2" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
     </row>
     <row r="251" spans="1:28" x14ac:dyDescent="0.2">
@@ -12880,10 +12787,10 @@
         <v>250</v>
       </c>
       <c r="B251" s="10" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C251" s="10" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="D251" t="s">
         <v>80</v>
@@ -12932,7 +12839,7 @@
         <v>59</v>
       </c>
       <c r="AB251" s="2" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
     </row>
     <row r="252" spans="1:28" x14ac:dyDescent="0.2">
@@ -12940,10 +12847,10 @@
         <v>251</v>
       </c>
       <c r="B252" s="10" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="C252" s="10" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="D252" t="s">
         <v>81</v>
@@ -12957,70 +12864,26 @@
       <c r="A253">
         <v>252</v>
       </c>
-      <c r="B253" s="10" t="s">
-        <v>545</v>
-      </c>
-      <c r="C253" s="10" t="s">
-        <v>546</v>
-      </c>
-      <c r="D253" t="s">
-        <v>80</v>
-      </c>
-      <c r="E253" s="9" t="d">
-        <v>2004-01-01</v>
-      </c>
-      <c r="F253" t="s">
-        <v>80</v>
-      </c>
-      <c r="G253" s="9" t="d">
-        <v>2001-05-01</v>
-      </c>
-      <c r="H253" s="9" t="d">
-        <v>2001-08-31</v>
-      </c>
-      <c r="I253" t="s">
-        <v>213</v>
-      </c>
-      <c r="J253">
-        <v>42.876917344577301</v>
-      </c>
-      <c r="K253">
-        <v>143.17406281821701</v>
-      </c>
-      <c r="L253">
-        <v>14</v>
-      </c>
-      <c r="Q253" t="s">
-        <v>49</v>
-      </c>
+      <c r="B253" s="10"/>
+      <c r="C253" s="10"/>
+      <c r="D253"/>
+      <c r="E253" s="9"/>
+      <c r="G253" s="9"/>
+      <c r="H253" s="9"/>
       <c r="R253"/>
-      <c r="S253">
-        <v>5</v>
-      </c>
-      <c r="T253">
-        <v>51.3</v>
-      </c>
-      <c r="U253">
-        <f>100-37.5</f>
-        <v>62.5</v>
-      </c>
-      <c r="Z253" t="s">
-        <v>25</v>
-      </c>
+      <c r="S253"/>
       <c r="AA253"/>
-      <c r="AB253" s="2" t="s">
-        <v>547</v>
-      </c>
+      <c r="AB253" s="2"/>
     </row>
     <row r="254" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>253</v>
       </c>
       <c r="B254" s="10" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="C254" s="10" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="D254" t="s">
         <v>81</v>
@@ -13035,10 +12898,10 @@
         <v>254</v>
       </c>
       <c r="B255" s="10" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="C255" s="10" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="D255" t="s">
         <v>81</v>
@@ -13053,10 +12916,10 @@
         <v>255</v>
       </c>
       <c r="B256" s="10" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="C256" s="10" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="D256" t="s">
         <v>81</v>
@@ -13071,10 +12934,10 @@
         <v>256</v>
       </c>
       <c r="B257" s="10" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="C257" s="10" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="D257" t="s">
         <v>81</v>
@@ -13089,10 +12952,10 @@
         <v>257</v>
       </c>
       <c r="B258" s="10" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="C258" s="10" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="D258" t="s">
         <v>81</v>
@@ -13107,10 +12970,10 @@
         <v>258</v>
       </c>
       <c r="B259" s="10" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="C259" s="10" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="D259" t="s">
         <v>81</v>
@@ -13125,10 +12988,10 @@
         <v>259</v>
       </c>
       <c r="B260" s="10" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="C260" s="10" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="D260" t="s">
         <v>81</v>
@@ -13143,10 +13006,10 @@
         <v>260</v>
       </c>
       <c r="B261" s="10" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="C261" s="10" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="D261" t="s">
         <v>81</v>
@@ -13161,10 +13024,10 @@
         <v>261</v>
       </c>
       <c r="B262" s="10" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="C262" s="10" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="D262" t="s">
         <v>81</v>
@@ -13179,10 +13042,10 @@
         <v>262</v>
       </c>
       <c r="B263" s="10" t="s">
-        <v>566</v>
+        <v>553</v>
       </c>
       <c r="C263" s="10" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="D263" t="s">
         <v>81</v>
@@ -13197,10 +13060,10 @@
         <v>263</v>
       </c>
       <c r="B264" s="10" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="C264" s="10" t="s">
-        <v>569</v>
+        <v>556</v>
       </c>
       <c r="D264" t="s">
         <v>81</v>
@@ -13215,10 +13078,10 @@
         <v>264</v>
       </c>
       <c r="B265" s="10" t="s">
-        <v>570</v>
+        <v>557</v>
       </c>
       <c r="C265" s="10" t="s">
-        <v>571</v>
+        <v>558</v>
       </c>
       <c r="D265" t="s">
         <v>81</v>
@@ -13233,10 +13096,10 @@
         <v>265</v>
       </c>
       <c r="B266" s="10" t="s">
-        <v>572</v>
+        <v>559</v>
       </c>
       <c r="C266" s="10" t="s">
-        <v>573</v>
+        <v>560</v>
       </c>
       <c r="D266" t="s">
         <v>81</v>
@@ -13251,10 +13114,10 @@
         <v>266</v>
       </c>
       <c r="B267" s="10" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="C267" s="10" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="D267" t="s">
         <v>81</v>
@@ -13269,10 +13132,10 @@
         <v>267</v>
       </c>
       <c r="B268" s="10" t="s">
-        <v>576</v>
+        <v>563</v>
       </c>
       <c r="C268" s="10" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="D268" t="s">
         <v>81</v>
@@ -13287,10 +13150,10 @@
         <v>268</v>
       </c>
       <c r="B269" s="10" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
       <c r="C269" s="10" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="D269" t="s">
         <v>81</v>
@@ -13305,10 +13168,10 @@
         <v>269</v>
       </c>
       <c r="B270" s="10" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="C270" s="10" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="D270" t="s">
         <v>81</v>
@@ -13323,10 +13186,10 @@
         <v>270</v>
       </c>
       <c r="B271" s="10" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="C271" s="10" t="s">
-        <v>583</v>
+        <v>570</v>
       </c>
       <c r="D271" t="s">
         <v>81</v>
@@ -13341,10 +13204,10 @@
         <v>271</v>
       </c>
       <c r="B272" s="10" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="C272" s="10" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="D272" t="s">
         <v>81</v>
@@ -13359,10 +13222,10 @@
         <v>272</v>
       </c>
       <c r="B273" s="10" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="C273" s="10" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="D273" t="s">
         <v>81</v>
@@ -13377,10 +13240,10 @@
         <v>273</v>
       </c>
       <c r="B274" s="10" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="C274" s="10" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="D274" t="s">
         <v>80</v>
@@ -13419,7 +13282,7 @@
       </c>
       <c r="AA274"/>
       <c r="AB274" s="2" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
     </row>
     <row r="275" spans="1:29" x14ac:dyDescent="0.2">
@@ -13427,10 +13290,10 @@
         <v>274</v>
       </c>
       <c r="B275" s="10" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="C275" s="10" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="D275" t="s">
         <v>80</v>
@@ -13469,7 +13332,7 @@
       </c>
       <c r="AA275"/>
       <c r="AB275" s="2" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
     </row>
     <row r="276" spans="1:29" x14ac:dyDescent="0.2">
@@ -13477,10 +13340,10 @@
         <v>275</v>
       </c>
       <c r="B276" s="10" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="C276" s="10" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="D276" t="s">
         <v>80</v>
@@ -13519,7 +13382,7 @@
       </c>
       <c r="AA276"/>
       <c r="AB276" s="2" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
     </row>
     <row r="277" spans="1:29" x14ac:dyDescent="0.2">
@@ -13527,10 +13390,10 @@
         <v>276</v>
       </c>
       <c r="B277" s="10" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
       <c r="C277" s="10" t="s">
-        <v>597</v>
+        <v>584</v>
       </c>
       <c r="D277" t="s">
         <v>80</v>
@@ -13540,10 +13403,10 @@
       <c r="S277"/>
       <c r="AA277"/>
       <c r="AB277" s="2" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="AC277" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="278" spans="1:29" x14ac:dyDescent="0.2">
@@ -13551,10 +13414,10 @@
         <v>277</v>
       </c>
       <c r="B278" s="10" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="C278" s="10" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="D278" t="s">
         <v>80</v>
@@ -13593,7 +13456,7 @@
       </c>
       <c r="AA278"/>
       <c r="AB278" s="2" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
     </row>
     <row r="279" spans="1:29" x14ac:dyDescent="0.2">
@@ -13601,10 +13464,10 @@
         <v>278</v>
       </c>
       <c r="B279" s="10" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="C279" s="10" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="D279" t="s">
         <v>80</v>
@@ -13643,7 +13506,7 @@
       </c>
       <c r="AA279"/>
       <c r="AB279" s="2" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
     </row>
     <row r="280" spans="1:29" x14ac:dyDescent="0.2">
@@ -13651,10 +13514,10 @@
         <v>279</v>
       </c>
       <c r="B280" s="10" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="C280" s="10" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="D280" t="s">
         <v>80</v>
@@ -13689,7 +13552,7 @@
       </c>
       <c r="AA280"/>
       <c r="AB280" s="2" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
     </row>
     <row r="281" spans="1:29" x14ac:dyDescent="0.2">
@@ -13697,10 +13560,10 @@
         <v>280</v>
       </c>
       <c r="B281" s="10" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="C281" s="10" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D281" t="s">
         <v>80</v>
@@ -13713,7 +13576,7 @@
       </c>
       <c r="G281"/>
       <c r="I281" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="J281">
         <v>20.654848210310298</v>
@@ -13754,7 +13617,7 @@
       </c>
       <c r="AA281"/>
       <c r="AB281" s="2" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
     </row>
     <row r="282" spans="1:29" x14ac:dyDescent="0.2">
@@ -13762,10 +13625,10 @@
         <v>281</v>
       </c>
       <c r="B282" s="10" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="C282" s="10" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="D282" t="s">
         <v>80</v>
@@ -13778,7 +13641,7 @@
       </c>
       <c r="G282"/>
       <c r="I282" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="J282">
         <v>19.423314723304902</v>
@@ -13819,7 +13682,7 @@
       </c>
       <c r="AA282"/>
       <c r="AB282" s="2" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
     </row>
     <row r="283" spans="1:29" x14ac:dyDescent="0.2">
@@ -13830,7 +13693,7 @@
         <v>146</v>
       </c>
       <c r="C283" s="10" t="s">
-        <v>766</v>
+        <v>747</v>
       </c>
       <c r="D283" t="s">
         <v>80</v>
@@ -13843,7 +13706,7 @@
       </c>
       <c r="G283"/>
       <c r="I283" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="J283">
         <v>20.654848210310298</v>
@@ -13884,7 +13747,7 @@
       </c>
       <c r="AA283"/>
       <c r="AB283" s="2" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
     </row>
     <row r="284" spans="1:29" x14ac:dyDescent="0.2">
@@ -13892,7 +13755,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="10" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="C284" s="10" t="s">
         <v>186</v>
@@ -13908,7 +13771,7 @@
       </c>
       <c r="G284"/>
       <c r="I284" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="J284">
         <v>20.654848210310298</v>
@@ -13951,7 +13814,7 @@
       </c>
       <c r="AA284"/>
       <c r="AB284" s="2" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
     </row>
     <row r="285" spans="1:29" x14ac:dyDescent="0.2">
@@ -13959,10 +13822,10 @@
         <v>284</v>
       </c>
       <c r="B285" s="10" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="C285" s="10" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D285" t="s">
         <v>80</v>
@@ -13975,7 +13838,7 @@
       </c>
       <c r="G285"/>
       <c r="I285" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="J285">
         <v>20.654848210310298</v>
@@ -14010,7 +13873,7 @@
       </c>
       <c r="AA285"/>
       <c r="AB285" s="2" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
     </row>
     <row r="286" spans="1:29" x14ac:dyDescent="0.2">
@@ -14018,10 +13881,10 @@
         <v>285</v>
       </c>
       <c r="B286" s="10" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="C286" s="10" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="D286" t="s">
         <v>80</v>
@@ -14077,7 +13940,7 @@
         <v>57</v>
       </c>
       <c r="AB286" s="2" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
     </row>
     <row r="287" spans="1:29" x14ac:dyDescent="0.2">
@@ -14085,10 +13948,10 @@
         <v>286</v>
       </c>
       <c r="B287" s="10" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="C287" s="10" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="D287" t="s">
         <v>80</v>
@@ -14131,7 +13994,7 @@
         <v>59</v>
       </c>
       <c r="AB287" s="2" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
     </row>
     <row r="288" spans="1:29" x14ac:dyDescent="0.2">
@@ -14139,10 +14002,10 @@
         <v>287</v>
       </c>
       <c r="B288" s="10" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="C288" s="10" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="D288" t="s">
         <v>80</v>
@@ -14188,7 +14051,7 @@
       </c>
       <c r="AA288"/>
       <c r="AB288" s="2" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
     </row>
     <row r="289" spans="1:28" x14ac:dyDescent="0.2">
@@ -14196,10 +14059,10 @@
         <v>288</v>
       </c>
       <c r="B289" s="10" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="C289" s="10" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="D289" t="s">
         <v>80</v>
@@ -14263,7 +14126,7 @@
         <v>57</v>
       </c>
       <c r="AB289" s="2" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
     </row>
     <row r="290" spans="1:28" x14ac:dyDescent="0.2">
@@ -14271,10 +14134,10 @@
         <v>289</v>
       </c>
       <c r="B290" s="10" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="C290" s="10" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="D290" t="s">
         <v>80</v>
@@ -14287,7 +14150,7 @@
       </c>
       <c r="G290"/>
       <c r="I290" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="J290">
         <v>0.317942587210643</v>
@@ -14330,7 +14193,7 @@
       </c>
       <c r="AA290"/>
       <c r="AB290" s="2" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
     </row>
     <row r="291" spans="1:28" x14ac:dyDescent="0.2">
@@ -14338,10 +14201,10 @@
         <v>290</v>
       </c>
       <c r="B291" s="10" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="C291" s="10" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="D291" t="s">
         <v>81</v>
@@ -14356,10 +14219,10 @@
         <v>291</v>
       </c>
       <c r="B292" s="10" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="C292" s="10" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="D292" t="s">
         <v>81</v>
@@ -14374,10 +14237,10 @@
         <v>292</v>
       </c>
       <c r="B293" s="10" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
       <c r="C293" s="10" t="s">
-        <v>626</v>
+        <v>613</v>
       </c>
       <c r="D293" t="s">
         <v>81</v>
@@ -14442,7 +14305,7 @@
         <v>59</v>
       </c>
       <c r="AB294" s="2" t="s">
-        <v>627</v>
+        <v>614</v>
       </c>
     </row>
     <row r="295" spans="1:28" x14ac:dyDescent="0.2">
@@ -14508,7 +14371,7 @@
         <v>59</v>
       </c>
       <c r="AB295" s="2" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
     </row>
     <row r="296" spans="1:28" x14ac:dyDescent="0.2">
@@ -14573,7 +14436,7 @@
         <v>59</v>
       </c>
       <c r="AB296" s="2" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
     </row>
     <row r="297" spans="1:28" x14ac:dyDescent="0.2">
@@ -14581,10 +14444,10 @@
         <v>296</v>
       </c>
       <c r="B297" s="10" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="C297" s="10" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
       <c r="D297" t="s">
         <v>81</v>
@@ -14599,10 +14462,10 @@
         <v>297</v>
       </c>
       <c r="B298" s="10" t="s">
-        <v>632</v>
+        <v>619</v>
       </c>
       <c r="C298" s="10" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="D298" t="s">
         <v>81</v>
@@ -14617,10 +14480,10 @@
         <v>298</v>
       </c>
       <c r="B299" s="10" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="C299" s="10" t="s">
-        <v>635</v>
+        <v>622</v>
       </c>
       <c r="D299" t="s">
         <v>81</v>
@@ -14635,10 +14498,10 @@
         <v>299</v>
       </c>
       <c r="B300" s="10" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="C300" s="10" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="D300" t="s">
         <v>81</v>
@@ -14652,15 +14515,9 @@
       <c r="A301">
         <v>300</v>
       </c>
-      <c r="B301" s="10" t="s">
-        <v>638</v>
-      </c>
-      <c r="C301" s="10" t="s">
-        <v>639</v>
-      </c>
-      <c r="D301" t="s">
-        <v>81</v>
-      </c>
+      <c r="B301" s="10"/>
+      <c r="C301" s="10"/>
+      <c r="D301"/>
       <c r="G301"/>
       <c r="R301"/>
       <c r="S301"/>
@@ -14671,10 +14528,10 @@
         <v>301</v>
       </c>
       <c r="B302" s="10" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="C302" s="10" t="s">
-        <v>641</v>
+        <v>626</v>
       </c>
       <c r="D302" t="s">
         <v>81</v>
@@ -14689,10 +14546,10 @@
         <v>302</v>
       </c>
       <c r="B303" s="10" t="s">
-        <v>642</v>
+        <v>627</v>
       </c>
       <c r="C303" s="10" t="s">
-        <v>643</v>
+        <v>628</v>
       </c>
       <c r="D303" t="s">
         <v>81</v>
@@ -14707,10 +14564,10 @@
         <v>303</v>
       </c>
       <c r="B304" s="10" t="s">
-        <v>644</v>
+        <v>629</v>
       </c>
       <c r="C304" s="10" t="s">
-        <v>645</v>
+        <v>630</v>
       </c>
       <c r="D304" t="s">
         <v>81</v>
@@ -14725,10 +14582,10 @@
         <v>304</v>
       </c>
       <c r="B305" s="10" t="s">
-        <v>646</v>
+        <v>631</v>
       </c>
       <c r="C305" s="10" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="D305" t="s">
         <v>81</v>
@@ -14743,10 +14600,10 @@
         <v>305</v>
       </c>
       <c r="B306" s="10" t="s">
-        <v>648</v>
+        <v>633</v>
       </c>
       <c r="C306" s="10" t="s">
-        <v>649</v>
+        <v>634</v>
       </c>
       <c r="D306" t="s">
         <v>81</v>
@@ -14761,10 +14618,10 @@
         <v>306</v>
       </c>
       <c r="B307" s="10" t="s">
-        <v>650</v>
+        <v>635</v>
       </c>
       <c r="C307" s="10" t="s">
-        <v>651</v>
+        <v>636</v>
       </c>
       <c r="D307" t="s">
         <v>81</v>
@@ -14778,15 +14635,9 @@
       <c r="A308">
         <v>307</v>
       </c>
-      <c r="B308" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="C308" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="D308" t="s">
-        <v>81</v>
-      </c>
+      <c r="B308" s="10"/>
+      <c r="C308" s="10"/>
+      <c r="D308"/>
       <c r="G308"/>
       <c r="R308"/>
       <c r="S308"/>
@@ -14797,10 +14648,10 @@
         <v>308</v>
       </c>
       <c r="B309" s="10" t="s">
-        <v>654</v>
+        <v>637</v>
       </c>
       <c r="C309" s="10" t="s">
-        <v>655</v>
+        <v>638</v>
       </c>
       <c r="D309" t="s">
         <v>81</v>
@@ -14815,10 +14666,10 @@
         <v>309</v>
       </c>
       <c r="B310" s="10" t="s">
-        <v>656</v>
+        <v>639</v>
       </c>
       <c r="C310" s="10" t="s">
-        <v>657</v>
+        <v>640</v>
       </c>
       <c r="D310" t="s">
         <v>81</v>
@@ -14833,10 +14684,10 @@
         <v>310</v>
       </c>
       <c r="B311" s="10" t="s">
-        <v>658</v>
+        <v>641</v>
       </c>
       <c r="C311" s="10" t="s">
-        <v>659</v>
+        <v>642</v>
       </c>
       <c r="D311" t="s">
         <v>81</v>
@@ -14851,10 +14702,10 @@
         <v>311</v>
       </c>
       <c r="B312" s="10" t="s">
-        <v>660</v>
+        <v>643</v>
       </c>
       <c r="C312" s="10" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="D312" t="s">
         <v>81</v>
@@ -14869,10 +14720,10 @@
         <v>312</v>
       </c>
       <c r="B313" s="10" t="s">
-        <v>662</v>
+        <v>645</v>
       </c>
       <c r="C313" s="10" t="s">
-        <v>663</v>
+        <v>646</v>
       </c>
       <c r="D313" t="s">
         <v>81</v>
@@ -14887,10 +14738,10 @@
         <v>313</v>
       </c>
       <c r="B314" s="10" t="s">
-        <v>664</v>
+        <v>647</v>
       </c>
       <c r="C314" s="10" t="s">
-        <v>665</v>
+        <v>648</v>
       </c>
       <c r="D314" t="s">
         <v>81</v>
@@ -14905,10 +14756,10 @@
         <v>314</v>
       </c>
       <c r="B315" s="10" t="s">
-        <v>666</v>
+        <v>649</v>
       </c>
       <c r="C315" s="10" t="s">
-        <v>667</v>
+        <v>650</v>
       </c>
       <c r="D315" t="s">
         <v>81</v>
@@ -14923,10 +14774,10 @@
         <v>315</v>
       </c>
       <c r="B316" s="10" t="s">
-        <v>668</v>
+        <v>651</v>
       </c>
       <c r="C316" s="10" t="s">
-        <v>669</v>
+        <v>652</v>
       </c>
       <c r="D316" t="s">
         <v>81</v>
@@ -14941,10 +14792,10 @@
         <v>316</v>
       </c>
       <c r="B317" s="10" t="s">
-        <v>670</v>
+        <v>653</v>
       </c>
       <c r="C317" s="10" t="s">
-        <v>671</v>
+        <v>654</v>
       </c>
       <c r="D317" t="s">
         <v>81</v>
@@ -14959,10 +14810,10 @@
         <v>317</v>
       </c>
       <c r="B318" s="10" t="s">
-        <v>672</v>
+        <v>655</v>
       </c>
       <c r="C318" s="10" t="s">
-        <v>673</v>
+        <v>656</v>
       </c>
       <c r="D318" t="s">
         <v>81</v>
@@ -14977,10 +14828,10 @@
         <v>318</v>
       </c>
       <c r="B319" s="10" t="s">
-        <v>674</v>
+        <v>657</v>
       </c>
       <c r="C319" s="10" t="s">
-        <v>675</v>
+        <v>658</v>
       </c>
       <c r="D319" t="s">
         <v>81</v>
@@ -14995,10 +14846,10 @@
         <v>319</v>
       </c>
       <c r="B320" s="10" t="s">
-        <v>676</v>
+        <v>659</v>
       </c>
       <c r="C320" s="10" t="s">
-        <v>677</v>
+        <v>660</v>
       </c>
       <c r="D320" t="s">
         <v>81</v>
@@ -15013,10 +14864,10 @@
         <v>320</v>
       </c>
       <c r="B321" s="10" t="s">
-        <v>678</v>
+        <v>661</v>
       </c>
       <c r="C321" s="10" t="s">
-        <v>679</v>
+        <v>662</v>
       </c>
       <c r="D321" t="s">
         <v>81</v>
@@ -15031,10 +14882,10 @@
         <v>321</v>
       </c>
       <c r="B322" s="10" t="s">
-        <v>680</v>
+        <v>663</v>
       </c>
       <c r="C322" s="10" t="s">
-        <v>681</v>
+        <v>664</v>
       </c>
       <c r="D322" t="s">
         <v>81</v>
@@ -15049,10 +14900,10 @@
         <v>322</v>
       </c>
       <c r="B323" s="10" t="s">
-        <v>682</v>
+        <v>665</v>
       </c>
       <c r="C323" s="10" t="s">
-        <v>683</v>
+        <v>666</v>
       </c>
       <c r="D323" t="s">
         <v>81</v>
@@ -15131,7 +14982,7 @@
       </c>
       <c r="AA324"/>
       <c r="AB324" s="2" t="s">
-        <v>684</v>
+        <v>667</v>
       </c>
     </row>
     <row r="325" spans="1:28" x14ac:dyDescent="0.2">
@@ -15139,10 +14990,10 @@
         <v>324</v>
       </c>
       <c r="B325" s="10" t="s">
-        <v>685</v>
+        <v>668</v>
       </c>
       <c r="C325" s="10" t="s">
-        <v>686</v>
+        <v>669</v>
       </c>
       <c r="D325" t="s">
         <v>81</v>
@@ -15160,10 +15011,10 @@
         <v>325</v>
       </c>
       <c r="B326" s="10" t="s">
-        <v>687</v>
+        <v>670</v>
       </c>
       <c r="C326" s="10" t="s">
-        <v>688</v>
+        <v>671</v>
       </c>
       <c r="D326" t="s">
         <v>81</v>
@@ -15178,10 +15029,10 @@
         <v>326</v>
       </c>
       <c r="B327" s="10" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
       <c r="C327" s="10" t="s">
-        <v>690</v>
+        <v>673</v>
       </c>
       <c r="D327" t="s">
         <v>81</v>
@@ -15196,10 +15047,10 @@
         <v>327</v>
       </c>
       <c r="B328" s="10" t="s">
-        <v>691</v>
+        <v>674</v>
       </c>
       <c r="C328" s="10" t="s">
-        <v>692</v>
+        <v>675</v>
       </c>
       <c r="D328" t="s">
         <v>81</v>
@@ -15214,10 +15065,10 @@
         <v>328</v>
       </c>
       <c r="B329" s="10" t="s">
-        <v>693</v>
+        <v>676</v>
       </c>
       <c r="C329" s="10" t="s">
-        <v>694</v>
+        <v>677</v>
       </c>
       <c r="D329" t="s">
         <v>81</v>
@@ -15233,10 +15084,10 @@
         <v>329</v>
       </c>
       <c r="B330" s="10" t="s">
-        <v>695</v>
+        <v>678</v>
       </c>
       <c r="C330" s="10" t="s">
-        <v>696</v>
+        <v>679</v>
       </c>
       <c r="D330" t="s">
         <v>81</v>
@@ -15251,10 +15102,10 @@
         <v>330</v>
       </c>
       <c r="B331" s="10" t="s">
-        <v>697</v>
+        <v>680</v>
       </c>
       <c r="C331" s="10" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
       <c r="D331" t="s">
         <v>81</v>
@@ -15269,10 +15120,10 @@
         <v>331</v>
       </c>
       <c r="B332" s="10" t="s">
-        <v>699</v>
+        <v>682</v>
       </c>
       <c r="C332" s="10" t="s">
-        <v>700</v>
+        <v>683</v>
       </c>
       <c r="D332" t="s">
         <v>81</v>
@@ -15287,10 +15138,10 @@
         <v>332</v>
       </c>
       <c r="B333" s="10" t="s">
-        <v>701</v>
+        <v>684</v>
       </c>
       <c r="C333" s="10" t="s">
-        <v>702</v>
+        <v>685</v>
       </c>
       <c r="D333" t="s">
         <v>81</v>
@@ -15306,10 +15157,10 @@
         <v>333</v>
       </c>
       <c r="B334" s="10" t="s">
-        <v>703</v>
+        <v>686</v>
       </c>
       <c r="C334" s="10" t="s">
-        <v>704</v>
+        <v>687</v>
       </c>
       <c r="D334" t="s">
         <v>81</v>
@@ -15324,10 +15175,10 @@
         <v>334</v>
       </c>
       <c r="B335" s="10" t="s">
-        <v>705</v>
+        <v>688</v>
       </c>
       <c r="C335" s="10" t="s">
-        <v>706</v>
+        <v>689</v>
       </c>
       <c r="D335" s="4" t="s">
         <v>81</v>
@@ -15338,10 +15189,10 @@
         <v>335</v>
       </c>
       <c r="B336" t="s">
-        <v>707</v>
+        <v>690</v>
       </c>
       <c r="C336" t="s">
-        <v>708</v>
+        <v>691</v>
       </c>
       <c r="D336" t="s">
         <v>80</v>
@@ -15354,7 +15205,7 @@
       </c>
       <c r="G336"/>
       <c r="I336" t="s">
-        <v>710</v>
+        <v>693</v>
       </c>
       <c r="J336">
         <v>5.8500917710755003</v>
@@ -15409,7 +15260,7 @@
         <v>64</v>
       </c>
       <c r="AB336" s="2" t="s">
-        <v>709</v>
+        <v>692</v>
       </c>
     </row>
     <row r="337" spans="1:28" x14ac:dyDescent="0.2">
@@ -15417,10 +15268,10 @@
         <v>336</v>
       </c>
       <c r="B337" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
       <c r="C337" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
       <c r="D337" t="s">
         <v>81</v>
@@ -15435,10 +15286,10 @@
         <v>337</v>
       </c>
       <c r="B338" t="s">
-        <v>713</v>
+        <v>696</v>
       </c>
       <c r="C338" t="s">
-        <v>714</v>
+        <v>697</v>
       </c>
       <c r="D338" t="s">
         <v>81</v>
@@ -15453,10 +15304,10 @@
         <v>338</v>
       </c>
       <c r="B339" t="s">
-        <v>715</v>
+        <v>698</v>
       </c>
       <c r="C339" t="s">
-        <v>716</v>
+        <v>699</v>
       </c>
       <c r="D339" t="s">
         <v>81</v>
@@ -15471,10 +15322,10 @@
         <v>339</v>
       </c>
       <c r="B340" t="s">
-        <v>717</v>
+        <v>700</v>
       </c>
       <c r="C340" t="s">
-        <v>718</v>
+        <v>701</v>
       </c>
       <c r="D340" t="s">
         <v>81</v>
@@ -15489,10 +15340,10 @@
         <v>340</v>
       </c>
       <c r="B341" t="s">
-        <v>719</v>
+        <v>702</v>
       </c>
       <c r="C341" t="s">
-        <v>720</v>
+        <v>703</v>
       </c>
       <c r="D341" t="s">
         <v>81</v>
@@ -15507,10 +15358,10 @@
         <v>341</v>
       </c>
       <c r="B342" t="s">
-        <v>721</v>
+        <v>704</v>
       </c>
       <c r="C342" t="s">
-        <v>722</v>
+        <v>705</v>
       </c>
       <c r="D342" t="s">
         <v>81</v>
@@ -15524,15 +15375,7 @@
       <c r="A343">
         <v>342</v>
       </c>
-      <c r="B343" t="s">
-        <v>723</v>
-      </c>
-      <c r="C343" t="s">
-        <v>724</v>
-      </c>
-      <c r="D343" t="s">
-        <v>81</v>
-      </c>
+      <c r="D343"/>
       <c r="G343"/>
       <c r="R343"/>
       <c r="S343"/>
@@ -15543,10 +15386,10 @@
         <v>343</v>
       </c>
       <c r="B344" t="s">
-        <v>725</v>
+        <v>706</v>
       </c>
       <c r="C344" t="s">
-        <v>726</v>
+        <v>707</v>
       </c>
       <c r="D344" t="s">
         <v>81</v>
@@ -15561,10 +15404,10 @@
         <v>344</v>
       </c>
       <c r="B345" t="s">
-        <v>727</v>
+        <v>708</v>
       </c>
       <c r="C345" t="s">
-        <v>728</v>
+        <v>709</v>
       </c>
       <c r="D345" t="s">
         <v>81</v>
@@ -15579,10 +15422,10 @@
         <v>345</v>
       </c>
       <c r="B346" t="s">
-        <v>729</v>
+        <v>710</v>
       </c>
       <c r="C346" t="s">
-        <v>730</v>
+        <v>711</v>
       </c>
       <c r="D346" t="s">
         <v>81</v>
@@ -15597,10 +15440,10 @@
         <v>346</v>
       </c>
       <c r="B347" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C347" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D347" t="s">
         <v>80</v>
@@ -15645,7 +15488,7 @@
         <v>59</v>
       </c>
       <c r="AB347" s="2" t="s">
-        <v>733</v>
+        <v>714</v>
       </c>
     </row>
     <row r="348" spans="1:28" x14ac:dyDescent="0.2">
@@ -15653,10 +15496,10 @@
         <v>347</v>
       </c>
       <c r="B348" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C348" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D348" t="s">
         <v>80</v>
@@ -15704,7 +15547,7 @@
         <v>25</v>
       </c>
       <c r="AB348" s="2" t="s">
-        <v>734</v>
+        <v>715</v>
       </c>
     </row>
     <row r="349" spans="1:28" x14ac:dyDescent="0.2">
@@ -15712,10 +15555,10 @@
         <v>348</v>
       </c>
       <c r="B349" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C349" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D349" t="s">
         <v>80</v>
@@ -15766,7 +15609,7 @@
         <v>9</v>
       </c>
       <c r="AB349" s="2" t="s">
-        <v>735</v>
+        <v>716</v>
       </c>
     </row>
     <row r="350" spans="1:28" x14ac:dyDescent="0.2">
@@ -15774,10 +15617,10 @@
         <v>349</v>
       </c>
       <c r="B350" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C350" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D350" t="s">
         <v>80</v>
@@ -15819,7 +15662,7 @@
         <v>13.483333333333334</v>
       </c>
       <c r="AB350" s="2" t="s">
-        <v>736</v>
+        <v>717</v>
       </c>
     </row>
     <row r="351" spans="1:28" x14ac:dyDescent="0.2">
@@ -15827,10 +15670,10 @@
         <v>350</v>
       </c>
       <c r="B351" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C351" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D351" t="s">
         <v>80</v>
@@ -15848,7 +15691,7 @@
         <v>1998-08-31</v>
       </c>
       <c r="I351" t="s">
-        <v>738</v>
+        <v>719</v>
       </c>
       <c r="J351">
         <v>46.886749967588898</v>
@@ -15883,7 +15726,7 @@
         <v>9</v>
       </c>
       <c r="AB351" s="2" t="s">
-        <v>737</v>
+        <v>718</v>
       </c>
     </row>
     <row r="352" spans="1:28" x14ac:dyDescent="0.2">
@@ -15891,10 +15734,10 @@
         <v>351</v>
       </c>
       <c r="B352" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C352" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D352" t="s">
         <v>80</v>
@@ -15907,7 +15750,7 @@
       </c>
       <c r="G352"/>
       <c r="I352" t="s">
-        <v>740</v>
+        <v>721</v>
       </c>
       <c r="J352">
         <v>39.222209747183399</v>
@@ -15941,7 +15784,7 @@
         <v>9</v>
       </c>
       <c r="AB352" s="2" t="s">
-        <v>739</v>
+        <v>720</v>
       </c>
     </row>
     <row r="353" spans="1:28" x14ac:dyDescent="0.2">
@@ -15949,10 +15792,10 @@
         <v>352</v>
       </c>
       <c r="B353" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C353" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D353" t="s">
         <v>80</v>
@@ -15970,7 +15813,7 @@
         <v>1997-04-30</v>
       </c>
       <c r="I353" t="s">
-        <v>742</v>
+        <v>723</v>
       </c>
       <c r="J353">
         <v>52.085287955897201</v>
@@ -16018,7 +15861,7 @@
         <v>9</v>
       </c>
       <c r="AB353" s="2" t="s">
-        <v>741</v>
+        <v>722</v>
       </c>
     </row>
     <row r="354" spans="1:28" x14ac:dyDescent="0.2">
@@ -16026,10 +15869,10 @@
         <v>353</v>
       </c>
       <c r="B354" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C354" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D354" t="s">
         <v>80</v>
@@ -16042,7 +15885,7 @@
       </c>
       <c r="G354"/>
       <c r="I354" t="s">
-        <v>744</v>
+        <v>725</v>
       </c>
       <c r="J354">
         <v>59.412843812069902</v>
@@ -16088,7 +15931,7 @@
         <v>9</v>
       </c>
       <c r="AB354" s="2" t="s">
-        <v>743</v>
+        <v>724</v>
       </c>
     </row>
     <row r="355" spans="1:28" x14ac:dyDescent="0.2">
@@ -16096,10 +15939,10 @@
         <v>354</v>
       </c>
       <c r="B355" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C355" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D355" t="s">
         <v>80</v>
@@ -16148,7 +15991,7 @@
         <v>9</v>
       </c>
       <c r="AB355" s="2" t="s">
-        <v>747</v>
+        <v>728</v>
       </c>
     </row>
     <row r="356" spans="1:28" x14ac:dyDescent="0.2">
@@ -16156,10 +15999,10 @@
         <v>355</v>
       </c>
       <c r="B356" t="s">
-        <v>745</v>
+        <v>726</v>
       </c>
       <c r="C356" t="s">
-        <v>746</v>
+        <v>727</v>
       </c>
       <c r="D356" t="s">
         <v>80</v>
@@ -16208,7 +16051,7 @@
         <v>9</v>
       </c>
       <c r="AB356" s="2" t="s">
-        <v>747</v>
+        <v>728</v>
       </c>
     </row>
     <row r="357" spans="1:28" x14ac:dyDescent="0.2">
@@ -16216,10 +16059,10 @@
         <v>356</v>
       </c>
       <c r="B357" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C357" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D357" t="s">
         <v>80</v>
@@ -16278,7 +16121,7 @@
         <v>9</v>
       </c>
       <c r="AB357" s="2" t="s">
-        <v>748</v>
+        <v>729</v>
       </c>
     </row>
     <row r="358" spans="1:28" x14ac:dyDescent="0.2">
@@ -16286,10 +16129,10 @@
         <v>357</v>
       </c>
       <c r="B358" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C358" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D358" t="s">
         <v>80</v>
@@ -16346,7 +16189,7 @@
         <v>9</v>
       </c>
       <c r="AB358" s="2" t="s">
-        <v>749</v>
+        <v>730</v>
       </c>
     </row>
     <row r="359" spans="1:28" x14ac:dyDescent="0.2">
@@ -16354,10 +16197,10 @@
         <v>358</v>
       </c>
       <c r="B359" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="C359" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="D359" t="s">
         <v>80</v>
@@ -16370,7 +16213,7 @@
       </c>
       <c r="G359"/>
       <c r="I359" t="s">
-        <v>751</v>
+        <v>732</v>
       </c>
       <c r="J359">
         <v>-33.269111880313197</v>
@@ -16410,7 +16253,7 @@
         <v>59</v>
       </c>
       <c r="AB359" s="2" t="s">
-        <v>750</v>
+        <v>731</v>
       </c>
     </row>
     <row r="360" spans="1:28" x14ac:dyDescent="0.2">
@@ -16418,10 +16261,10 @@
         <v>359</v>
       </c>
       <c r="B360" t="s">
-        <v>753</v>
+        <v>734</v>
       </c>
       <c r="C360" t="s">
-        <v>754</v>
+        <v>735</v>
       </c>
       <c r="D360" t="s">
         <v>81</v>
@@ -16436,10 +16279,10 @@
         <v>360</v>
       </c>
       <c r="B361" t="s">
-        <v>755</v>
+        <v>736</v>
       </c>
       <c r="C361" t="s">
-        <v>756</v>
+        <v>737</v>
       </c>
       <c r="D361" t="s">
         <v>81</v>
@@ -16454,10 +16297,10 @@
         <v>361</v>
       </c>
       <c r="B362" t="s">
-        <v>757</v>
+        <v>738</v>
       </c>
       <c r="C362" t="s">
-        <v>758</v>
+        <v>739</v>
       </c>
       <c r="D362" t="s">
         <v>81</v>
@@ -16472,10 +16315,10 @@
         <v>362</v>
       </c>
       <c r="B363" t="s">
-        <v>759</v>
+        <v>740</v>
       </c>
       <c r="C363" t="s">
-        <v>760</v>
+        <v>741</v>
       </c>
       <c r="D363" t="s">
         <v>81</v>
@@ -16490,10 +16333,10 @@
         <v>363</v>
       </c>
       <c r="B364" t="s">
-        <v>761</v>
+        <v>742</v>
       </c>
       <c r="C364" t="s">
-        <v>762</v>
+        <v>743</v>
       </c>
       <c r="D364" t="s">
         <v>81</v>
@@ -16508,10 +16351,10 @@
         <v>364</v>
       </c>
       <c r="B365" t="s">
-        <v>763</v>
+        <v>744</v>
       </c>
       <c r="C365" t="s">
-        <v>764</v>
+        <v>745</v>
       </c>
       <c r="D365" t="s">
         <v>81</v>
@@ -16525,7 +16368,7 @@
         <v>365</v>
       </c>
       <c r="B366" t="s">
-        <v>767</v>
+        <v>748</v>
       </c>
       <c r="C366" t="s">
         <v>103</v>
@@ -16574,7 +16417,7 @@
         <v>366</v>
       </c>
       <c r="B367" t="s">
-        <v>768</v>
+        <v>749</v>
       </c>
       <c r="C367" t="s">
         <v>104</v>
@@ -16623,7 +16466,7 @@
         <v>367</v>
       </c>
       <c r="B368" t="s">
-        <v>767</v>
+        <v>748</v>
       </c>
       <c r="C368" t="s">
         <v>103</v>
@@ -16669,7 +16512,7 @@
         <v>368</v>
       </c>
       <c r="B369" t="s">
-        <v>768</v>
+        <v>749</v>
       </c>
       <c r="C369" t="s">
         <v>104</v>
@@ -18061,54 +17904,53 @@
     <hyperlink ref="AB249" r:id="rId26" xr:uid="{1A7C9939-AD98-874F-8A61-9F244AA95EE8}"/>
     <hyperlink ref="AB250" r:id="rId27" xr:uid="{FAC05E73-7C57-AD4E-AF01-1EDA760337B8}"/>
     <hyperlink ref="AB251" r:id="rId28" xr:uid="{262A1CE8-D62F-7D4F-A208-85A4FB2CE4F9}"/>
-    <hyperlink ref="AB253" r:id="rId29" xr:uid="{FDC771C2-B35B-7645-9564-8E1B377E85D4}"/>
-    <hyperlink ref="AB274" r:id="rId30" tooltip="Persistent link using digital object identifier" xr:uid="{57670D07-3D8C-F54A-BECB-A1E8EE4C75A7}"/>
-    <hyperlink ref="AB275" r:id="rId31" tooltip="Persistent link using digital object identifier" xr:uid="{4A0D79BD-6F59-AD4A-BDD3-46BB39633252}"/>
-    <hyperlink ref="AB276" r:id="rId32" tooltip="Persistent link using digital object identifier" xr:uid="{92BEAC71-A8AB-6A49-9959-E0F718A87551}"/>
-    <hyperlink ref="AB277" r:id="rId33" xr:uid="{274173AF-BCA4-404F-A4C5-BFAFAAC49C89}"/>
-    <hyperlink ref="AB278" r:id="rId34" xr:uid="{FB4AFF34-D1B9-1B46-A573-A058082C9E7A}"/>
-    <hyperlink ref="AB279" r:id="rId35" xr:uid="{CDF40199-3A1C-7D4D-98BA-6F02CE481263}"/>
-    <hyperlink ref="AB280" r:id="rId36" xr:uid="{2CDCC7A0-3D12-594D-9860-4EADA4D2844C}"/>
-    <hyperlink ref="AB281" r:id="rId37" xr:uid="{4ECEB60B-0CE5-1742-8A60-B2C6E4F55288}"/>
-    <hyperlink ref="AB282" r:id="rId38" xr:uid="{FCE030C1-5735-5E4F-B943-A4EAD694E483}"/>
-    <hyperlink ref="AB283" r:id="rId39" xr:uid="{74703F21-DF1D-7542-96D4-775F246A6B8C}"/>
-    <hyperlink ref="AB284" r:id="rId40" xr:uid="{0970A517-4F33-0B41-A886-3D5A7357F99B}"/>
-    <hyperlink ref="AB285" r:id="rId41" xr:uid="{EAF0E2CD-35A6-C74D-AD17-BE123EEC83DB}"/>
-    <hyperlink ref="AB286" r:id="rId42" tooltip="Persistent link using digital object identifier" xr:uid="{4C3A6908-0F8F-B349-A55E-124E99CDF570}"/>
-    <hyperlink ref="AB287" r:id="rId43" xr:uid="{5F4D9B03-C72C-D24A-859C-63155B4DCE2C}"/>
-    <hyperlink ref="AB288" r:id="rId44" xr:uid="{BE431EA2-E8A3-7D4B-B340-51E61B8BF0F8}"/>
-    <hyperlink ref="AB289" r:id="rId45" xr:uid="{3FE77E55-FC21-2941-AB46-2498DFCB44E9}"/>
-    <hyperlink ref="AB290" r:id="rId46" xr:uid="{B45923DF-8BF3-0E4E-B3F0-6BEBDD5B6B1C}"/>
-    <hyperlink ref="AB58" r:id="rId47" xr:uid="{9EE3E1BD-B480-C34D-8D86-40842D1F0437}"/>
-    <hyperlink ref="AB49" r:id="rId48" xr:uid="{A29E0B3B-9B09-B24E-B796-745EE174D532}"/>
-    <hyperlink ref="AB48" r:id="rId49" xr:uid="{C1589CFF-DB3D-AD4E-85DC-25BEB81BC2C4}"/>
-    <hyperlink ref="AB294" r:id="rId50" tooltip="Persistent link using digital object identifier" xr:uid="{6A0BA7C1-B1A8-3D4C-9FB6-551FDA431F36}"/>
-    <hyperlink ref="AB295" r:id="rId51" tooltip="Persistent link using digital object identifier" xr:uid="{E702884B-D3D5-DF47-AE62-1C2953BFC054}"/>
-    <hyperlink ref="AB296" r:id="rId52" xr:uid="{F799773D-85C8-7944-8D46-AE063DAC6A06}"/>
-    <hyperlink ref="AB115" r:id="rId53" xr:uid="{8F138AC6-3594-3349-A561-CA5C387D8468}"/>
-    <hyperlink ref="AB324" r:id="rId54" tooltip="Persistent link using digital object identifier" xr:uid="{BC578F07-8E6F-2E4B-A2D9-85A5FD16F655}"/>
-    <hyperlink ref="AB336" r:id="rId55" xr:uid="{99FC54FC-43F4-8B49-B8E6-386CC41046A6}"/>
-    <hyperlink ref="AB347" r:id="rId56" xr:uid="{BED8E7CB-1FD7-504F-9F5B-7BF7FA27312C}"/>
-    <hyperlink ref="AB348" r:id="rId57" xr:uid="{84F989AC-201F-124E-9423-A953878A2D0C}"/>
-    <hyperlink ref="AB349" r:id="rId58" xr:uid="{578B4CD6-093A-A04A-A20F-A3ECE8499446}"/>
-    <hyperlink ref="AB350" r:id="rId59" tooltip="Persistent link using digital object identifier" xr:uid="{6A3151FA-7747-8949-843D-6DF06FEE3BA8}"/>
-    <hyperlink ref="AB351" r:id="rId60" tooltip="Persistent link using digital object identifier" xr:uid="{D88F6D46-5EB8-DF46-B075-464B769F7122}"/>
-    <hyperlink ref="AB352" r:id="rId61" xr:uid="{5C05107B-0788-2946-854D-21CEB66B7391}"/>
-    <hyperlink ref="AB353" r:id="rId62" tooltip="Persistent link using digital object identifier" xr:uid="{B9C3C0C0-9324-EE4B-8EB4-03C148B85536}"/>
-    <hyperlink ref="AB354" r:id="rId63" xr:uid="{D4788405-5B4B-0A43-A2B9-CED4C78BEE10}"/>
-    <hyperlink ref="AB355" r:id="rId64" xr:uid="{40DDB605-EB6B-654B-9870-81DC6EF88AEE}"/>
-    <hyperlink ref="AB356" r:id="rId65" xr:uid="{AB51C033-527B-7D43-B3D6-8C0EA82BF0C2}"/>
-    <hyperlink ref="AB357" r:id="rId66" tooltip="Persistent link using digital object identifier" xr:uid="{FC0652EF-1A7D-384F-9E2E-DDDD29314ACB}"/>
-    <hyperlink ref="AB358" r:id="rId67" xr:uid="{A7371822-B12A-FC48-8F6A-3DEAD6E966B5}"/>
-    <hyperlink ref="AB359" r:id="rId68" tooltip="Persistent link using digital object identifier" xr:uid="{BEC32A03-2C4E-F54E-8888-6F5758D66FEB}"/>
-    <hyperlink ref="AB62" r:id="rId69" xr:uid="{84FCF329-42E3-D041-A512-E4025EAF21D4}"/>
-    <hyperlink ref="AB63" r:id="rId70" xr:uid="{4BAD4B3E-2A74-BB4B-82BC-96D7FC6C08C5}"/>
-    <hyperlink ref="AB34" r:id="rId71" xr:uid="{3BD02AA7-AD77-5A41-885D-97B6E200B1A7}"/>
-    <hyperlink ref="AB35" r:id="rId72" xr:uid="{BD621737-5DAB-3D41-887F-6F06F8C43C1E}"/>
-    <hyperlink ref="AB366" r:id="rId73" xr:uid="{B9886E10-ACAD-BC4B-A250-086FA135BEEC}"/>
-    <hyperlink ref="AB367" r:id="rId74" xr:uid="{AD739A70-632C-3340-ADC3-A9D8440C1F45}"/>
-    <hyperlink ref="AB368" r:id="rId75" xr:uid="{E49934A6-CD48-E54B-AD3F-914A756C8CB0}"/>
-    <hyperlink ref="AB369" r:id="rId76" xr:uid="{5D39ADC3-C3B6-5246-A907-706937F4AE72}"/>
+    <hyperlink ref="AB274" r:id="rId29" tooltip="Persistent link using digital object identifier" xr:uid="{57670D07-3D8C-F54A-BECB-A1E8EE4C75A7}"/>
+    <hyperlink ref="AB275" r:id="rId30" tooltip="Persistent link using digital object identifier" xr:uid="{4A0D79BD-6F59-AD4A-BDD3-46BB39633252}"/>
+    <hyperlink ref="AB276" r:id="rId31" tooltip="Persistent link using digital object identifier" xr:uid="{92BEAC71-A8AB-6A49-9959-E0F718A87551}"/>
+    <hyperlink ref="AB277" r:id="rId32" xr:uid="{274173AF-BCA4-404F-A4C5-BFAFAAC49C89}"/>
+    <hyperlink ref="AB278" r:id="rId33" xr:uid="{FB4AFF34-D1B9-1B46-A573-A058082C9E7A}"/>
+    <hyperlink ref="AB279" r:id="rId34" xr:uid="{CDF40199-3A1C-7D4D-98BA-6F02CE481263}"/>
+    <hyperlink ref="AB280" r:id="rId35" xr:uid="{2CDCC7A0-3D12-594D-9860-4EADA4D2844C}"/>
+    <hyperlink ref="AB281" r:id="rId36" xr:uid="{4ECEB60B-0CE5-1742-8A60-B2C6E4F55288}"/>
+    <hyperlink ref="AB282" r:id="rId37" xr:uid="{FCE030C1-5735-5E4F-B943-A4EAD694E483}"/>
+    <hyperlink ref="AB283" r:id="rId38" xr:uid="{74703F21-DF1D-7542-96D4-775F246A6B8C}"/>
+    <hyperlink ref="AB284" r:id="rId39" xr:uid="{0970A517-4F33-0B41-A886-3D5A7357F99B}"/>
+    <hyperlink ref="AB285" r:id="rId40" xr:uid="{EAF0E2CD-35A6-C74D-AD17-BE123EEC83DB}"/>
+    <hyperlink ref="AB286" r:id="rId41" tooltip="Persistent link using digital object identifier" xr:uid="{4C3A6908-0F8F-B349-A55E-124E99CDF570}"/>
+    <hyperlink ref="AB287" r:id="rId42" xr:uid="{5F4D9B03-C72C-D24A-859C-63155B4DCE2C}"/>
+    <hyperlink ref="AB288" r:id="rId43" xr:uid="{BE431EA2-E8A3-7D4B-B340-51E61B8BF0F8}"/>
+    <hyperlink ref="AB289" r:id="rId44" xr:uid="{3FE77E55-FC21-2941-AB46-2498DFCB44E9}"/>
+    <hyperlink ref="AB290" r:id="rId45" xr:uid="{B45923DF-8BF3-0E4E-B3F0-6BEBDD5B6B1C}"/>
+    <hyperlink ref="AB58" r:id="rId46" xr:uid="{9EE3E1BD-B480-C34D-8D86-40842D1F0437}"/>
+    <hyperlink ref="AB49" r:id="rId47" xr:uid="{A29E0B3B-9B09-B24E-B796-745EE174D532}"/>
+    <hyperlink ref="AB48" r:id="rId48" xr:uid="{C1589CFF-DB3D-AD4E-85DC-25BEB81BC2C4}"/>
+    <hyperlink ref="AB294" r:id="rId49" tooltip="Persistent link using digital object identifier" xr:uid="{6A0BA7C1-B1A8-3D4C-9FB6-551FDA431F36}"/>
+    <hyperlink ref="AB295" r:id="rId50" tooltip="Persistent link using digital object identifier" xr:uid="{E702884B-D3D5-DF47-AE62-1C2953BFC054}"/>
+    <hyperlink ref="AB296" r:id="rId51" xr:uid="{F799773D-85C8-7944-8D46-AE063DAC6A06}"/>
+    <hyperlink ref="AB115" r:id="rId52" xr:uid="{8F138AC6-3594-3349-A561-CA5C387D8468}"/>
+    <hyperlink ref="AB324" r:id="rId53" tooltip="Persistent link using digital object identifier" xr:uid="{BC578F07-8E6F-2E4B-A2D9-85A5FD16F655}"/>
+    <hyperlink ref="AB336" r:id="rId54" xr:uid="{99FC54FC-43F4-8B49-B8E6-386CC41046A6}"/>
+    <hyperlink ref="AB347" r:id="rId55" xr:uid="{BED8E7CB-1FD7-504F-9F5B-7BF7FA27312C}"/>
+    <hyperlink ref="AB348" r:id="rId56" xr:uid="{84F989AC-201F-124E-9423-A953878A2D0C}"/>
+    <hyperlink ref="AB349" r:id="rId57" xr:uid="{578B4CD6-093A-A04A-A20F-A3ECE8499446}"/>
+    <hyperlink ref="AB350" r:id="rId58" tooltip="Persistent link using digital object identifier" xr:uid="{6A3151FA-7747-8949-843D-6DF06FEE3BA8}"/>
+    <hyperlink ref="AB351" r:id="rId59" tooltip="Persistent link using digital object identifier" xr:uid="{D88F6D46-5EB8-DF46-B075-464B769F7122}"/>
+    <hyperlink ref="AB352" r:id="rId60" xr:uid="{5C05107B-0788-2946-854D-21CEB66B7391}"/>
+    <hyperlink ref="AB353" r:id="rId61" tooltip="Persistent link using digital object identifier" xr:uid="{B9C3C0C0-9324-EE4B-8EB4-03C148B85536}"/>
+    <hyperlink ref="AB354" r:id="rId62" xr:uid="{D4788405-5B4B-0A43-A2B9-CED4C78BEE10}"/>
+    <hyperlink ref="AB355" r:id="rId63" xr:uid="{40DDB605-EB6B-654B-9870-81DC6EF88AEE}"/>
+    <hyperlink ref="AB356" r:id="rId64" xr:uid="{AB51C033-527B-7D43-B3D6-8C0EA82BF0C2}"/>
+    <hyperlink ref="AB357" r:id="rId65" tooltip="Persistent link using digital object identifier" xr:uid="{FC0652EF-1A7D-384F-9E2E-DDDD29314ACB}"/>
+    <hyperlink ref="AB358" r:id="rId66" xr:uid="{A7371822-B12A-FC48-8F6A-3DEAD6E966B5}"/>
+    <hyperlink ref="AB359" r:id="rId67" tooltip="Persistent link using digital object identifier" xr:uid="{BEC32A03-2C4E-F54E-8888-6F5758D66FEB}"/>
+    <hyperlink ref="AB62" r:id="rId68" xr:uid="{84FCF329-42E3-D041-A512-E4025EAF21D4}"/>
+    <hyperlink ref="AB63" r:id="rId69" xr:uid="{4BAD4B3E-2A74-BB4B-82BC-96D7FC6C08C5}"/>
+    <hyperlink ref="AB34" r:id="rId70" xr:uid="{3BD02AA7-AD77-5A41-885D-97B6E200B1A7}"/>
+    <hyperlink ref="AB35" r:id="rId71" xr:uid="{BD621737-5DAB-3D41-887F-6F06F8C43C1E}"/>
+    <hyperlink ref="AB366" r:id="rId72" xr:uid="{B9886E10-ACAD-BC4B-A250-086FA135BEEC}"/>
+    <hyperlink ref="AB367" r:id="rId73" xr:uid="{AD739A70-632C-3340-ADC3-A9D8440C1F45}"/>
+    <hyperlink ref="AB368" r:id="rId74" xr:uid="{E49934A6-CD48-E54B-AD3F-914A756C8CB0}"/>
+    <hyperlink ref="AB369" r:id="rId75" xr:uid="{5D39ADC3-C3B6-5246-A907-706937F4AE72}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>